<commit_message>
Create admin file deletion services
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -336,15 +336,15 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.13"/>

</xml_diff>

<commit_message>
Cache invalidation for all menus endpoint
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -279,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,6 +314,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -333,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,6 +631,9 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Revert "Cache invalidation for all menus endpoint"
This reverts commit 7a826dfc89f27bda7eb7fbb1808912dc649ade11.
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -279,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,10 +314,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -337,10 +333,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10:F18"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,9 +627,6 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9"/>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>